<commit_message>
Database Window and Viewer fixed, also added Delete Record button.
</commit_message>
<xml_diff>
--- a/Test Reports/2222_test.xlsx
+++ b/Test Reports/2222_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,263 +424,176 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Test ID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Test ID</t>
+          <t>Collection Date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Sample Collection Date</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Latitude</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Longitude</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Area (ha)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Area (ha)</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Mobile No.</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Mobile No.</t>
+          <t>Soil pH</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Soil pH</t>
+          <t>Nitrogen</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Nitrogen</t>
+          <t>Phosphorus</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Phosphorus</t>
+          <t>Potassium</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Potassium</t>
+          <t>Electrical Conductivity</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Electrical Conductivity</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Temperature</t>
+          <t>Moisture</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Moisture</t>
+          <t>Humidity</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>Humidity</t>
+          <t>Soil Health Score</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Soil Health Score</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Crop Recommendations</t>
+          <t>Recommendations</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>148</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2222</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>15-03-2024</t>
-        </is>
+          <t>12-03-2024</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>253</v>
       </c>
       <c r="D2" t="n">
-        <v>2536</v>
-      </c>
-      <c r="E2" t="n">
-        <v>25445</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>sdakjsdkajsd</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" t="inlineStr">
+        <v>256</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>asdasdasdasdasd</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="H2" t="n">
         <v>26</v>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>26a5sd5646as5d</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>265a6s5dasd</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>9865623232</t>
-        </is>
+          <t>2323265589</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>7</v>
       </c>
       <c r="L2" t="n">
-        <v>2.3</v>
+        <v>250</v>
       </c>
       <c r="M2" t="n">
+        <v>120</v>
+      </c>
+      <c r="N2" t="n">
         <v>200</v>
       </c>
-      <c r="N2" t="n">
-        <v>150</v>
-      </c>
       <c r="O2" t="n">
-        <v>222</v>
+        <v>2</v>
       </c>
       <c r="P2" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="R2" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="S2" t="n">
-        <v>40</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.4559054912895061</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>149</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2222</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>15-03-2024</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2536</v>
-      </c>
-      <c r="E3" t="n">
-        <v>25445</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>sdakjsdkajsd</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>26</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>265a6s5dasd</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>9865623232</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="M3" t="n">
-        <v>200</v>
-      </c>
-      <c r="N3" t="n">
-        <v>150</v>
-      </c>
-      <c r="O3" t="n">
-        <v>222</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>25</v>
-      </c>
-      <c r="R3" t="n">
-        <v>33</v>
-      </c>
-      <c r="S3" t="n">
-        <v>40</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.4559054912895061</v>
-      </c>
-      <c r="U3" t="inlineStr">
+        <v>0.5473459137758564</v>
+      </c>
+      <c r="T2" t="inlineStr">
         <is>
           <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
         </is>

</xml_diff>